<commit_message>
Add order to the label
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -127,10 +127,7 @@
     <t>Wind Energy Project Life-cycle Phase</t>
   </si>
   <si>
-    <t>wpl:0.Identification</t>
-  </si>
-  <si>
-    <t>Identification</t>
+    <t>1 Identification</t>
   </si>
   <si>
     <t>Initial stage where potential wind energy sites are identified based on criteria like wind resource, land availability, and environmental factors.</t>
@@ -139,91 +136,73 @@
     <t>Screening, Site Selection, Pilot Study</t>
   </si>
   <si>
-    <t>wpl:1.Feasibility</t>
+    <t>2 Feasibility</t>
+  </si>
+  <si>
+    <t>Detailed analysis of the identified site, including technical, environmental, and financial assessments to determine project viability.</t>
+  </si>
+  <si>
+    <t>3 Development</t>
+  </si>
+  <si>
+    <t>Preparation of detailed plans and engineering designs, wind turbine technology and vendor selection, securing permits, land leases, financing, and stakeholder agreements required to move forward with the project.</t>
+  </si>
+  <si>
+    <t>Design, Planning &amp; Permitting</t>
+  </si>
+  <si>
+    <t>4 Pre-Construction</t>
+  </si>
+  <si>
+    <t>Finalizing detailed engineering designs, procurement of materials, and preparation of the site for construction, including contractor selection.</t>
+  </si>
+  <si>
+    <t>Purchase, Procurement</t>
+  </si>
+  <si>
+    <t>5 Construction</t>
+  </si>
+  <si>
+    <t>Physical construction of the wind farm, including infrastructure setup (turbines, roads, electrical connections) and project management oversight.</t>
+  </si>
+  <si>
+    <t>6  Commissioning</t>
+  </si>
+  <si>
+    <t>Testing and certifying that the wind farm operates according to design specifications before becoming fully operational.</t>
+  </si>
+  <si>
+    <t>7 Operation &amp; Maintenance</t>
+  </si>
+  <si>
+    <t>Ongoing operation of the wind farm, including regular monitoring, maintenance, and optimization to ensure maximum energy production and efficiency.</t>
+  </si>
+  <si>
+    <t>Middle of life</t>
+  </si>
+  <si>
+    <t>8 Decommissioning</t>
+  </si>
+  <si>
+    <t>End-of-life activities for the wind farm, involving dismantling turbines and infrastructure, restoring the site, and recycling or disposing of materials.</t>
+  </si>
+  <si>
+    <t>End of life</t>
+  </si>
+  <si>
+    <t>Reference Project Life-cycle Phase</t>
+  </si>
+  <si>
+    <t>Project phase is a collection of logically related project activities (processes) that culminates in the completion of one or more deliverables. Project Life Cycle is the series of phases that a project passes through from its start to its completion.</t>
+  </si>
+  <si>
+    <t>https://www.pmi.org/</t>
+  </si>
+  <si>
+    <t>urn:ISBN:9781628256659</t>
   </si>
   <si>
     <t>Feasibility</t>
-  </si>
-  <si>
-    <t>Detailed analysis of the identified site, including technical, environmental, and financial assessments to determine project viability.</t>
-  </si>
-  <si>
-    <t>wpl:2.Development</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>Preparation of detailed plans and engineering designs, wind turbine technology and vendor selection, securing permits, land leases, financing, and stakeholder agreements required to move forward with the project.</t>
-  </si>
-  <si>
-    <t>Design, Planning &amp; Permitting</t>
-  </si>
-  <si>
-    <t>wpl:3.Pre-Construction</t>
-  </si>
-  <si>
-    <t>Pre-Construction</t>
-  </si>
-  <si>
-    <t>Finalizing detailed engineering designs, procurement of materials, and preparation of the site for construction, including contractor selection.</t>
-  </si>
-  <si>
-    <t>Purchase, Procurement</t>
-  </si>
-  <si>
-    <t>wpl:4.Construction</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Physical construction of the wind farm, including infrastructure setup (turbines, roads, electrical connections) and project management oversight.</t>
-  </si>
-  <si>
-    <t>wpl:5.Commissioning</t>
-  </si>
-  <si>
-    <t>Commissioning</t>
-  </si>
-  <si>
-    <t>Testing and certifying that the wind farm operates according to design specifications before becoming fully operational.</t>
-  </si>
-  <si>
-    <t>wpl:6.Operation-Maintenance</t>
-  </si>
-  <si>
-    <t>Operation &amp; Maintenance</t>
-  </si>
-  <si>
-    <t>Ongoing operation of the wind farm, including regular monitoring, maintenance, and optimization to ensure maximum energy production and efficiency.</t>
-  </si>
-  <si>
-    <t>Middle of life</t>
-  </si>
-  <si>
-    <t>wpl:7.Decommissioning</t>
-  </si>
-  <si>
-    <t>Decommissioning</t>
-  </si>
-  <si>
-    <t>End-of-life activities for the wind farm, involving dismantling turbines and infrastructure, restoring the site, and recycling or disposing of materials.</t>
-  </si>
-  <si>
-    <t>End of life</t>
-  </si>
-  <si>
-    <t>Reference Project Life-cycle Phase</t>
-  </si>
-  <si>
-    <t>Project phase is a collection of logically related project activities (processes) that culminates in the completion of one or more deliverables. Project Life Cycle is the series of phases that a project passes through from its start to its completion.</t>
-  </si>
-  <si>
-    <t>https://www.pmi.org/</t>
-  </si>
-  <si>
-    <t>urn:ISBN:9781628256659</t>
   </si>
   <si>
     <t>This phase determines if the business case is valid and if the organization has the capability to deliver the intended outcome.</t>
@@ -1081,7 +1060,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
-        <f t="shared" ref="A16:A17" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A16:A51" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>wpl:LifeCyclePhase</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -1125,17 +1104,18 @@
       <c r="N17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:1Identification</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>41</v>
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" ref="E18:E25" si="2">$A$17</f>
@@ -1152,14 +1132,15 @@
       <c r="N18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:2Feasibility</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="4" t="str">
@@ -1177,17 +1158,18 @@
       <c r="N19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:3Development</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>48</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1204,17 +1186,18 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>49</v>
+      <c r="A21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:4Pre-Construction</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1231,14 +1214,15 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>53</v>
+      <c r="A22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:5Construction</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="4" t="str">
@@ -1256,14 +1240,15 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>56</v>
+      <c r="A23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:6Commissioning</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="4" t="str">
@@ -1281,17 +1266,18 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>59</v>
+      <c r="A24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:7Operation-Maintenance</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1308,17 +1294,18 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>63</v>
+      <c r="A25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>wpl:8Decommissioning</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1336,14 +1323,14 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="str">
-        <f t="shared" ref="A26:A51" si="3">IF(ISBLANK($B26),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B26," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="1"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="4" t="str">
@@ -1354,11 +1341,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1366,29 +1353,29 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Feasibility</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="4" t="str">
-        <f t="shared" ref="E27:E33" si="4">$A$26</f>
+        <f t="shared" ref="E27:E33" si="3">$A$26</f>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1396,29 +1383,29 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Design</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1426,29 +1413,29 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Build</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1456,29 +1443,29 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Test</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1486,29 +1473,29 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Deploy</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1516,29 +1503,29 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Close</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1546,16 +1533,16 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:AllProjectPhases</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="16"/>
       <c r="E33" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>wpl:ReferenceProjectLife-cyclePhase</v>
       </c>
       <c r="F33" s="3"/>
@@ -1570,11 +1557,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="16"/>
@@ -1594,16 +1581,16 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Conception</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="16"/>
       <c r="E35" s="4" t="str">
-        <f t="shared" ref="E35:E39" si="5">$A$34</f>
+        <f t="shared" ref="E35:E39" si="4">$A$34</f>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="F35" s="3"/>
@@ -1618,16 +1605,16 @@
     </row>
     <row r="36">
       <c r="A36" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Design</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="16"/>
       <c r="E36" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="F36" s="3"/>
@@ -1642,16 +1629,16 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Realisation</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="16"/>
       <c r="E37" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="F37" s="3"/>
@@ -1666,16 +1653,16 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Service</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="16"/>
       <c r="E38" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="F38" s="3"/>
@@ -1690,16 +1677,16 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:AllProductPhases</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="16"/>
       <c r="E39" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>wpl:ProductLife-cyclePhase</v>
       </c>
       <c r="F39" s="3"/>
@@ -1714,11 +1701,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Process</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
@@ -1735,20 +1722,20 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:ProductProcess</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E41" s="4" t="str">
-        <f t="shared" ref="E41:E42" si="6">A40</f>
+        <f t="shared" ref="E41:E42" si="5">A40</f>
         <v>wpl:Process</v>
       </c>
       <c r="F41" s="3"/>
@@ -1763,16 +1750,16 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:WindTurbineProductProcess</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="16"/>
       <c r="E42" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>wpl:ProductProcess</v>
       </c>
       <c r="F42" s="3"/>
@@ -1787,11 +1774,11 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:WindPowerPlantProcess</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
@@ -1811,14 +1798,14 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:ProjectManagementProcess</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="4" t="str">
@@ -1837,17 +1824,17 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:SupportingProcess</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E45" s="4" t="str">
         <f>A40</f>
@@ -1865,14 +1852,14 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="4"/>
@@ -1880,11 +1867,11 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -1892,29 +1879,29 @@
     </row>
     <row r="47">
       <c r="A47" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Initiation</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="4" t="str">
-        <f t="shared" ref="E47:E51" si="7">$A$46</f>
+        <f t="shared" ref="E47:E51" si="6">$A$46</f>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -1922,29 +1909,29 @@
     </row>
     <row r="48">
       <c r="A48" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Planning</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -1952,31 +1939,31 @@
     </row>
     <row r="49">
       <c r="A49" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Execution</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E49" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -1984,29 +1971,29 @@
     </row>
     <row r="50">
       <c r="A50" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Performance-Control</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
@@ -2014,29 +2001,29 @@
     </row>
     <row r="51">
       <c r="A51" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>wpl:Closure</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>wpl:ProcessGroup</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
@@ -2715,7 +2702,6 @@
     </row>
     <row r="145">
       <c r="A145" s="3"/>
-      <c r="B145" s="21"/>
     </row>
     <row r="146">
       <c r="A146" s="3"/>
@@ -2742,14 +2728,14 @@
     </row>
     <row r="153">
       <c r="A153" s="3" t="str">
-        <f t="shared" ref="A153:A154" si="8">IF(ISBLANK($B153),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B153," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A153:A154" si="7">IF(ISBLANK($B153),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B153," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v/>
       </c>
       <c r="B153" s="21"/>
     </row>
     <row r="154">
       <c r="A154" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>

</xml_diff>